<commit_message>
kati 1 ob 3 done
</commit_message>
<xml_diff>
--- a/2966-3/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-3-Ferizaj-Armendi-leg.xlsx
+++ b/2966-3/3-Katet/regjistri/29-Koordinatat-e-kateve-2966-3-Ferizaj-Armendi-leg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Ferizaj\Ingjinierike\2966-1-Ferizaj-Armendi-leg\2966-3\3-Katet\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031CE788-6852-45EC-9C6C-7DFA8B19FE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB7CEEC-41E2-4475-A386-1BFB64E6D7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="255" windowWidth="27930" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$56</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
   <si>
     <t>Y</t>
   </si>
@@ -1244,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="B14:I27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B30:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,13 +1726,13 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C31" s="5">
-        <v>7510648.7396</v>
+        <v>7510657.7807</v>
       </c>
       <c r="D31" s="5">
-        <v>4693483.1380000003</v>
+        <v>4693488.7863999996</v>
       </c>
       <c r="E31" s="10">
         <v>651.38900000000001</v>
@@ -1747,18 +1747,18 @@
         <v>16</v>
       </c>
       <c r="I31" s="27">
-        <v>79.843999999999994</v>
+        <v>77.703999999999994</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C32" s="5">
-        <v>7510648.5892000003</v>
+        <v>7510657.5647999998</v>
       </c>
       <c r="D32" s="5">
-        <v>4693483.0460999999</v>
+        <v>4693488.6553999996</v>
       </c>
       <c r="E32" s="10">
         <v>651.38900000000001</v>
@@ -1770,15 +1770,15 @@
       <c r="H32" s="27"/>
       <c r="I32" s="27"/>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C33" s="5">
-        <v>7510641.7006000001</v>
+        <v>7510650.6701999996</v>
       </c>
       <c r="D33" s="5">
-        <v>4693478.8332000002</v>
+        <v>4693484.4735000003</v>
       </c>
       <c r="E33" s="10">
         <v>651.38900000000001</v>
@@ -1790,15 +1790,15 @@
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C34" s="5">
-        <v>7510653.6935999999</v>
+        <v>7510662.5954999998</v>
       </c>
       <c r="D34" s="5">
-        <v>4693474.8667000001</v>
+        <v>4693480.5250000004</v>
       </c>
       <c r="E34" s="10">
         <v>651.38900000000001</v>
@@ -1810,15 +1810,15 @@
       <c r="H34" s="27"/>
       <c r="I34" s="27"/>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C35" s="5">
-        <v>7510649.8039999995</v>
+        <v>7510658.7253</v>
       </c>
       <c r="D35" s="5">
-        <v>4693472.3590000002</v>
+        <v>4693478.0266000004</v>
       </c>
       <c r="E35" s="10">
         <v>651.38900000000001</v>
@@ -1830,15 +1830,15 @@
       <c r="H35" s="27"/>
       <c r="I35" s="27"/>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C36" s="5">
-        <v>7510648.0659999996</v>
+        <v>7510656.9850000003</v>
       </c>
       <c r="D36" s="5">
-        <v>4693471.3150000004</v>
+        <v>4693476.9709999999</v>
       </c>
       <c r="E36" s="10">
         <v>651.38900000000001</v>
@@ -1850,15 +1850,15 @@
       <c r="H36" s="27"/>
       <c r="I36" s="27"/>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C37" s="5">
-        <v>7510648.0179000003</v>
+        <v>7510658.6602999996</v>
       </c>
       <c r="D37" s="5">
-        <v>4693471.3956000004</v>
+        <v>4693478.1381000001</v>
       </c>
       <c r="E37" s="10">
         <v>651.38900000000001</v>
@@ -1870,15 +1870,15 @@
       <c r="H37" s="27"/>
       <c r="I37" s="27"/>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C38" s="5">
-        <v>7510646.6425000001</v>
+        <v>7510655.1160000004</v>
       </c>
       <c r="D38" s="5">
-        <v>4693470.5544999996</v>
+        <v>4693477.1179999998</v>
       </c>
       <c r="E38" s="10">
         <v>651.38900000000001</v>
@@ -1889,22 +1889,16 @@
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
       <c r="I38" s="27"/>
-      <c r="Q38">
-        <v>98.998000000000005</v>
-      </c>
-      <c r="R38">
-        <v>15.858000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C39" s="5">
-        <v>7510649.7476000004</v>
+        <v>7510656.4336000001</v>
       </c>
       <c r="D39" s="5">
-        <v>4693472.4534999998</v>
+        <v>4693477.9172</v>
       </c>
       <c r="E39" s="10">
         <v>651.38900000000001</v>
@@ -1917,18 +1911,18 @@
         <v>14</v>
       </c>
       <c r="I39" s="10">
-        <v>8.3149999999999995</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+        <v>8.6590000000000007</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C40" s="5">
-        <v>7510641.1344999997</v>
+        <v>7510650.1025</v>
       </c>
       <c r="D40" s="5">
-        <v>4693479.7813999997</v>
+        <v>4693485.4210999999</v>
       </c>
       <c r="E40" s="10">
         <v>651.38900000000001</v>
@@ -1939,19 +1933,16 @@
       <c r="G40" s="27"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
-      <c r="Q40">
-        <v>98.998000000000005</v>
-      </c>
-    </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C41" s="5">
-        <v>7510648.0900999997</v>
+        <v>7510657.0235000001</v>
       </c>
       <c r="D41" s="5">
-        <v>4693483.8622000003</v>
+        <v>4693489.5478999997</v>
       </c>
       <c r="E41" s="10">
         <v>651.38900000000001</v>
@@ -1965,13 +1956,10 @@
       </c>
       <c r="I41" s="14">
         <f>SUM(I31:I39)</f>
-        <v>88.158999999999992</v>
-      </c>
-      <c r="Q41">
-        <v>15.858000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
+        <v>86.363</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D42" s="6"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -1979,7 +1967,7 @@
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D43" s="6"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
@@ -1987,7 +1975,7 @@
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="13" t="s">
         <v>5</v>
       </c>
@@ -2013,18 +2001,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="11">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C45" s="5">
-        <v>7510641.693</v>
+        <v>7510650.6589000002</v>
       </c>
       <c r="D45" s="5">
-        <v>4693478.8720000004</v>
+        <v>4693484.4923</v>
       </c>
       <c r="E45" s="10">
-        <v>645.96799999999996</v>
+        <v>645.94299999999998</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>20</v>
@@ -2036,18 +2024,18 @@
         <v>21</v>
       </c>
       <c r="I45" s="27">
-        <v>50.45</v>
-      </c>
-    </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+        <v>50.09</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="11">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C46" s="5">
-        <v>7510648.1128000002</v>
+        <v>7510657.1150000002</v>
       </c>
       <c r="D46" s="5">
-        <v>4693482.6546999998</v>
+        <v>4693488.3409000002</v>
       </c>
       <c r="E46" s="10">
         <v>645.94299999999998</v>
@@ -2059,18 +2047,18 @@
       <c r="H46" s="27"/>
       <c r="I46" s="27"/>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="11">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C47" s="5">
-        <v>7510648.0619999999</v>
+        <v>7510657.0719999997</v>
       </c>
       <c r="D47" s="5">
-        <v>4693482.7410000004</v>
+        <v>4693488.4129999997</v>
       </c>
       <c r="E47" s="10">
-        <v>645.86400000000003</v>
+        <v>646.09199999999998</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>20</v>
@@ -2079,15 +2067,15 @@
       <c r="H47" s="27"/>
       <c r="I47" s="27"/>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="11">
-        <v>115</v>
+        <v>17</v>
       </c>
       <c r="C48" s="5">
-        <v>7510644.0905999998</v>
+        <v>7510659.7607000005</v>
       </c>
       <c r="D48" s="5">
-        <v>4693474.8295</v>
+        <v>4693489.9873000002</v>
       </c>
       <c r="E48" s="10">
         <v>645.94299999999998</v>
@@ -2101,13 +2089,13 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" s="11">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="C49" s="5">
-        <v>7510653.2237</v>
+        <v>7510662.1574999997</v>
       </c>
       <c r="D49" s="5">
-        <v>4693480.2110000001</v>
+        <v>4693485.8748000003</v>
       </c>
       <c r="E49" s="10">
         <v>645.94299999999998</v>
@@ -2116,18 +2104,18 @@
         <v>20</v>
       </c>
       <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B50" s="11">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C50" s="5">
-        <v>7510648.5768999998</v>
+        <v>7510653.0743000004</v>
       </c>
       <c r="D50" s="5">
-        <v>4693483.1991999997</v>
+        <v>4693480.4605</v>
       </c>
       <c r="E50" s="10">
         <v>645.94299999999998</v>
@@ -2136,140 +2124,100 @@
         <v>20</v>
       </c>
       <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
+      <c r="H50" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="14">
+        <f>SUM(I45:I48)</f>
+        <v>50.09</v>
+      </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="11">
-        <v>119</v>
-      </c>
-      <c r="C51" s="5">
-        <v>7510648.6446000002</v>
-      </c>
-      <c r="D51" s="5">
-        <v>4693483.0843000002</v>
-      </c>
-      <c r="E51" s="10">
-        <v>645.94299999999998</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G51" s="27"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="11">
-        <v>124</v>
-      </c>
-      <c r="C52" s="5">
-        <v>7510650.6882999996</v>
-      </c>
-      <c r="D52" s="5">
-        <v>4693484.4433000004</v>
-      </c>
-      <c r="E52" s="10">
-        <v>645.94299999999998</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G52" s="27"/>
-      <c r="H52" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I52" s="14">
-        <f>SUM(I45:I50)</f>
-        <v>50.45</v>
-      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D53" s="6"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D54" s="6"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D55" s="6"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+    </row>
+    <row r="54" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="41"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I55" s="37"/>
+      <c r="J55" s="31"/>
+      <c r="K55" s="32"/>
     </row>
     <row r="56" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K56" s="1"/>
+      <c r="A56" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="44"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="46">
+        <v>140</v>
+      </c>
+      <c r="F56" s="47"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="39"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="34"/>
     </row>
     <row r="57" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="F57" s="41"/>
-      <c r="G57" s="42"/>
-      <c r="H57" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="I57" s="37"/>
-      <c r="J57" s="31"/>
-      <c r="K57" s="32"/>
-    </row>
-    <row r="58" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58" s="44"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="46">
-        <v>140</v>
-      </c>
-      <c r="F58" s="47"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="34"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K58" s="1"/>
     </row>
     <row r="59" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K60" s="1"/>
-    </row>
-    <row r="61" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="K61" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J57:K58"/>
+    <mergeCell ref="J55:K56"/>
     <mergeCell ref="A3:K6"/>
-    <mergeCell ref="H57:I58"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="H55:I56"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="E56:G56"/>
     <mergeCell ref="G31:G41"/>
     <mergeCell ref="H31:H38"/>
     <mergeCell ref="I31:I38"/>
-    <mergeCell ref="G45:G52"/>
-    <mergeCell ref="H45:H50"/>
-    <mergeCell ref="I45:I50"/>
+    <mergeCell ref="G45:G50"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="I45:I48"/>
     <mergeCell ref="A1:K2"/>
     <mergeCell ref="C8:J10"/>
     <mergeCell ref="G15:G27"/>

</xml_diff>